<commit_message>
Updated Excel sheet with better model names and made figure larger
</commit_message>
<xml_diff>
--- a/DietEstimates.xlsx
+++ b/DietEstimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amikk\Documents\Rprojects\Diet-sensitivty-to-TDFs-and-priors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6342231-E4A5-440D-9782-504ADBA1116E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79C9A74-4DFE-43E0-8DB1-F30F98E0EA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{313E8A8B-1F62-40B3-8FFB-18833A481903}"/>
+    <workbookView xWindow="43890" yWindow="270" windowWidth="28800" windowHeight="15300" xr2:uid="{313E8A8B-1F62-40B3-8FFB-18833A481903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,12 +72,6 @@
     <t>Felicetti</t>
   </si>
   <si>
-    <t>MikkelsenMin1</t>
-  </si>
-  <si>
-    <t>MikkelsenPlus1</t>
-  </si>
-  <si>
     <t>Ro</t>
   </si>
   <si>
@@ -97,6 +91,12 @@
   </si>
   <si>
     <t>Dmodel</t>
+  </si>
+  <si>
+    <t>Mikkelsen-1</t>
+  </si>
+  <si>
+    <t>Mikkelsen+1</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,16 +478,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -502,10 +502,10 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -993,11 +993,11 @@
         <v>3</v>
       </c>
       <c r="B17" s="2">
-        <f>B2-1</f>
+        <f t="shared" ref="B17:C21" si="0">B2-1</f>
         <v>3.62</v>
       </c>
       <c r="C17" s="2">
-        <f>C2-1</f>
+        <f t="shared" si="0"/>
         <v>3.87</v>
       </c>
       <c r="D17" s="2">
@@ -1013,7 +1013,7 @@
         <v>0.245</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
@@ -1027,11 +1027,11 @@
         <v>4</v>
       </c>
       <c r="B18" s="2">
-        <f>B3-1</f>
+        <f t="shared" si="0"/>
         <v>5.64</v>
       </c>
       <c r="C18" s="2">
-        <f>C3-1</f>
+        <f t="shared" si="0"/>
         <v>4.28</v>
       </c>
       <c r="D18" s="2">
@@ -1047,7 +1047,7 @@
         <v>0.191</v>
       </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I18" s="2">
         <v>2</v>
@@ -1061,11 +1061,11 @@
         <v>5</v>
       </c>
       <c r="B19" s="2">
-        <f>B4-1</f>
+        <f t="shared" si="0"/>
         <v>4.07</v>
       </c>
       <c r="C19" s="2">
-        <f>C4-1</f>
+        <f t="shared" si="0"/>
         <v>4.6100000000000003</v>
       </c>
       <c r="D19" s="2">
@@ -1081,7 +1081,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="H19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I19" s="2">
         <v>3</v>
@@ -1095,11 +1095,11 @@
         <v>6</v>
       </c>
       <c r="B20" s="2">
-        <f>B5-1</f>
+        <f t="shared" si="0"/>
         <v>4.1900000000000004</v>
       </c>
       <c r="C20" s="2">
-        <f>C5-1</f>
+        <f t="shared" si="0"/>
         <v>4.45</v>
       </c>
       <c r="D20" s="2">
@@ -1115,7 +1115,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="H20" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I20" s="2">
         <v>4</v>
@@ -1129,11 +1129,11 @@
         <v>7</v>
       </c>
       <c r="B21" s="2">
-        <f>B6-1</f>
+        <f t="shared" si="0"/>
         <v>4.04</v>
       </c>
       <c r="C21" s="2">
-        <f>C6-1</f>
+        <f t="shared" si="0"/>
         <v>3.84</v>
       </c>
       <c r="D21" s="2">
@@ -1149,7 +1149,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="H21" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I21" s="2">
         <v>5</v>
@@ -1163,11 +1163,11 @@
         <v>3</v>
       </c>
       <c r="B22" s="2">
-        <f>B2+1</f>
+        <f t="shared" ref="B22:C26" si="1">B2+1</f>
         <v>5.62</v>
       </c>
       <c r="C22" s="2">
-        <f>C2+1</f>
+        <f t="shared" si="1"/>
         <v>5.87</v>
       </c>
       <c r="D22" s="2">
@@ -1183,7 +1183,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I22" s="2">
         <v>1</v>
@@ -1197,11 +1197,11 @@
         <v>4</v>
       </c>
       <c r="B23" s="2">
-        <f>B3+1</f>
+        <f t="shared" si="1"/>
         <v>7.64</v>
       </c>
       <c r="C23" s="2">
-        <f>C3+1</f>
+        <f t="shared" si="1"/>
         <v>6.28</v>
       </c>
       <c r="D23" s="2">
@@ -1217,7 +1217,7 @@
         <v>0.83499999999999996</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I23" s="2">
         <v>2</v>
@@ -1231,11 +1231,11 @@
         <v>5</v>
       </c>
       <c r="B24" s="2">
-        <f>B4+1</f>
+        <f t="shared" si="1"/>
         <v>6.07</v>
       </c>
       <c r="C24" s="2">
-        <f>C4+1</f>
+        <f t="shared" si="1"/>
         <v>6.61</v>
       </c>
       <c r="D24" s="2">
@@ -1251,7 +1251,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="H24" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I24" s="2">
         <v>3</v>
@@ -1265,11 +1265,11 @@
         <v>6</v>
       </c>
       <c r="B25" s="2">
-        <f>B5+1</f>
+        <f t="shared" si="1"/>
         <v>6.19</v>
       </c>
       <c r="C25" s="2">
-        <f>C5+1</f>
+        <f t="shared" si="1"/>
         <v>6.45</v>
       </c>
       <c r="D25" s="2">
@@ -1285,7 +1285,7 @@
         <v>0.17399999999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I25" s="2">
         <v>4</v>
@@ -1299,11 +1299,11 @@
         <v>7</v>
       </c>
       <c r="B26" s="2">
-        <f>B6+1</f>
+        <f t="shared" si="1"/>
         <v>6.04</v>
       </c>
       <c r="C26" s="2">
-        <f>C6+1</f>
+        <f t="shared" si="1"/>
         <v>5.84</v>
       </c>
       <c r="D26" s="2">
@@ -1319,7 +1319,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="H26" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I26" s="2">
         <v>5</v>
@@ -1351,7 +1351,7 @@
         <v>0.99399999999999999</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I27" s="2">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I28" s="2">
         <v>2</v>
@@ -1415,7 +1415,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I29" s="2">
         <v>3</v>
@@ -1447,7 +1447,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="H30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I30" s="2">
         <v>4</v>
@@ -1479,7 +1479,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I31" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Wrote .Rmd to compare effect of priors
</commit_message>
<xml_diff>
--- a/DietEstimates.xlsx
+++ b/DietEstimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amikk\Documents\Rprojects\Diet-sensitivty-to-TDFs-and-priors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79C9A74-4DFE-43E0-8DB1-F30F98E0EA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253D9BEC-79E1-4A36-98B0-CDE0309080A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43890" yWindow="270" windowWidth="28800" windowHeight="15300" xr2:uid="{313E8A8B-1F62-40B3-8FFB-18833A481903}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed description of methods and changed plots to bar charts
</commit_message>
<xml_diff>
--- a/DietEstimates.xlsx
+++ b/DietEstimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amikk\Documents\Rprojects\Diet-sensitivty-to-TDFs-and-priors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253D9BEC-79E1-4A36-98B0-CDE0309080A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6B9E19-A748-459E-AB67-CE908BC42726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43890" yWindow="270" windowWidth="28800" windowHeight="15300" xr2:uid="{313E8A8B-1F62-40B3-8FFB-18833A481903}"/>
+    <workbookView xWindow="46680" yWindow="480" windowWidth="28800" windowHeight="15300" xr2:uid="{313E8A8B-1F62-40B3-8FFB-18833A481903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,21 +45,6 @@
     <t>UCI</t>
   </si>
   <si>
-    <t>ants</t>
-  </si>
-  <si>
-    <t>bilberry</t>
-  </si>
-  <si>
-    <t>crowberry</t>
-  </si>
-  <si>
-    <t>lingonberry</t>
-  </si>
-  <si>
-    <t>moose</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -97,6 +82,21 @@
   </si>
   <si>
     <t>Mikkelsen+1</t>
+  </si>
+  <si>
+    <t>Ants</t>
+  </si>
+  <si>
+    <t>Bilberry</t>
+  </si>
+  <si>
+    <t>Crowberry</t>
+  </si>
+  <si>
+    <t>Lingonberry</t>
+  </si>
+  <si>
+    <t>Moose</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,16 +478,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -499,18 +499,18 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>4.62</v>
@@ -531,7 +531,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2">
         <v>6.64</v>
@@ -563,7 +563,7 @@
         <v>0.499</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I3" s="2">
         <v>2</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
         <v>5.07</v>
@@ -595,7 +595,7 @@
         <v>0.17299999999999999</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I4" s="2">
         <v>3</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2">
         <v>5.19</v>
@@ -627,7 +627,7 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I5" s="2">
         <v>4</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>5.04</v>
@@ -659,7 +659,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I6" s="2">
         <v>5</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2">
         <v>4.8869999999999996</v>
@@ -691,7 +691,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>6.8979999999999997</v>
@@ -723,7 +723,7 @@
         <v>0.61399999999999999</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I8" s="2">
         <v>2</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>5.3230000000000004</v>
@@ -755,7 +755,7 @@
         <v>0.104</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I9" s="2">
         <v>3</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
         <v>5.4509999999999996</v>
@@ -787,7 +787,7 @@
         <v>0.27</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I10" s="2">
         <v>4</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
         <v>5.3029999999999999</v>
@@ -819,7 +819,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I11" s="2">
         <v>5</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
         <v>4.3579999999999997</v>
@@ -851,7 +851,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
         <v>6.3780000000000001</v>
@@ -883,7 +883,7 @@
         <v>0.39800000000000002</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I13" s="2">
         <v>2</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>4.8079999999999998</v>
@@ -915,7 +915,7 @@
         <v>0.23200000000000001</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I14" s="2">
         <v>3</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
         <v>4.931</v>
@@ -947,7 +947,7 @@
         <v>0.377</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I15" s="2">
         <v>4</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>4.7830000000000004</v>
@@ -979,7 +979,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I16" s="2">
         <v>5</v>
@@ -990,14 +990,14 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17:C21" si="0">B2-1</f>
+        <f>B2-1</f>
         <v>3.62</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="0"/>
+        <f>C2-1</f>
         <v>3.87</v>
       </c>
       <c r="D17" s="2">
@@ -1013,7 +1013,7 @@
         <v>0.245</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
@@ -1024,14 +1024,14 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" si="0"/>
+        <f>B3-1</f>
         <v>5.64</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="0"/>
+        <f>C3-1</f>
         <v>4.28</v>
       </c>
       <c r="D18" s="2">
@@ -1047,7 +1047,7 @@
         <v>0.191</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I18" s="2">
         <v>2</v>
@@ -1058,14 +1058,14 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" si="0"/>
+        <f>B4-1</f>
         <v>4.07</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="0"/>
+        <f>C4-1</f>
         <v>4.6100000000000003</v>
       </c>
       <c r="D19" s="2">
@@ -1081,7 +1081,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I19" s="2">
         <v>3</v>
@@ -1092,14 +1092,14 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="0"/>
+        <f>B5-1</f>
         <v>4.1900000000000004</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="0"/>
+        <f>C5-1</f>
         <v>4.45</v>
       </c>
       <c r="D20" s="2">
@@ -1115,7 +1115,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I20" s="2">
         <v>4</v>
@@ -1126,14 +1126,14 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" si="0"/>
+        <f>B6-1</f>
         <v>4.04</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="0"/>
+        <f>C6-1</f>
         <v>3.84</v>
       </c>
       <c r="D21" s="2">
@@ -1149,7 +1149,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I21" s="2">
         <v>5</v>
@@ -1160,14 +1160,14 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" ref="B22:C26" si="1">B2+1</f>
+        <f>B2+1</f>
         <v>5.62</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="1"/>
+        <f>C2+1</f>
         <v>5.87</v>
       </c>
       <c r="D22" s="2">
@@ -1183,7 +1183,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I22" s="2">
         <v>1</v>
@@ -1194,14 +1194,14 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="1"/>
+        <f>B3+1</f>
         <v>7.64</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="1"/>
+        <f>C3+1</f>
         <v>6.28</v>
       </c>
       <c r="D23" s="2">
@@ -1217,7 +1217,7 @@
         <v>0.83499999999999996</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I23" s="2">
         <v>2</v>
@@ -1228,14 +1228,14 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" si="1"/>
+        <f>B4+1</f>
         <v>6.07</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="1"/>
+        <f>C4+1</f>
         <v>6.61</v>
       </c>
       <c r="D24" s="2">
@@ -1251,7 +1251,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="H24" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I24" s="2">
         <v>3</v>
@@ -1262,14 +1262,14 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="1"/>
+        <f>B5+1</f>
         <v>6.19</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="1"/>
+        <f>C5+1</f>
         <v>6.45</v>
       </c>
       <c r="D25" s="2">
@@ -1285,7 +1285,7 @@
         <v>0.17399999999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I25" s="2">
         <v>4</v>
@@ -1296,14 +1296,14 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="1"/>
+        <f>B6+1</f>
         <v>6.04</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="1"/>
+        <f>C6+1</f>
         <v>5.84</v>
       </c>
       <c r="D26" s="2">
@@ -1319,7 +1319,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I26" s="2">
         <v>5</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         <v>0.99399999999999999</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I27" s="2">
         <v>1</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -1383,7 +1383,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="H28" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I28" s="2">
         <v>2</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
@@ -1415,7 +1415,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H29" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I29" s="2">
         <v>3</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
@@ -1447,7 +1447,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="H30" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I30" s="2">
         <v>4</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="H31" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I31" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Ddi more work answering committe questions, seperated my bears by sex and compared siet estimates between them
</commit_message>
<xml_diff>
--- a/DietEstimates.xlsx
+++ b/DietEstimates.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amikk\Documents\Rprojects\Diet-sensitivty-to-TDFs-and-priors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6B9E19-A748-459E-AB67-CE908BC42726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07476FCC-8378-417A-B6DF-E44888C8ED32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46680" yWindow="480" windowWidth="28800" windowHeight="15300" xr2:uid="{313E8A8B-1F62-40B3-8FFB-18833A481903}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{313E8A8B-1F62-40B3-8FFB-18833A481903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,7 +104,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,13 +124,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,15 +155,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +483,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,28 +527,28 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>4.62</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>4.87</v>
       </c>
-      <c r="D2" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E2" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F2" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="G2" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F2" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="2">
@@ -541,28 +559,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>6.64</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>5.28</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="E3" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F3" s="2">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.499</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F3" s="4">
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="2">
@@ -573,28 +591,28 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>5.07</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>5.61</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D4" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.154</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2">
@@ -605,28 +623,28 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
         <v>5.19</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>5.45</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="E5" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="F5" s="2">
-        <v>0.247</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="F5" s="4">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.314</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="2">
@@ -637,28 +655,28 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2">
-        <v>5.04</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4.84</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="B6" s="4">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="D6" s="4">
         <v>0.04</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F6" s="2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="F6" s="4">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="2">
@@ -673,13 +691,13 @@
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>4.8869999999999996</v>
+        <v>4.87</v>
       </c>
       <c r="C7" s="2">
         <v>4.6280000000000001</v>
       </c>
       <c r="D7" s="2">
-        <v>0.08</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E7" s="2">
         <v>6.0000000000000001E-3</v>
@@ -705,22 +723,22 @@
         <v>17</v>
       </c>
       <c r="B8" s="2">
-        <v>6.8979999999999997</v>
+        <v>6.899</v>
       </c>
       <c r="C8" s="2">
         <v>4.9939999999999998</v>
       </c>
       <c r="D8" s="2">
-        <v>0.58699999999999997</v>
+        <v>0.622</v>
       </c>
       <c r="E8" s="2">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>0.56100000000000005</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="G8" s="2">
-        <v>0.61399999999999999</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
@@ -737,22 +755,22 @@
         <v>18</v>
       </c>
       <c r="B9" s="2">
-        <v>5.3230000000000004</v>
+        <v>5.327</v>
       </c>
       <c r="C9" s="2">
         <v>5.2910000000000004</v>
       </c>
       <c r="D9" s="2">
-        <v>6.3E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E9" s="2">
         <v>0.02</v>
       </c>
       <c r="F9" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>0.104</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="H9" t="s">
         <v>5</v>
@@ -775,16 +793,16 @@
         <v>5.149</v>
       </c>
       <c r="D10" s="2">
-        <v>0.223</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="E10" s="2">
-        <v>2.4E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>0.17499999999999999</v>
+        <v>0.153</v>
       </c>
       <c r="G10" s="2">
-        <v>0.27</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
@@ -801,22 +819,22 @@
         <v>20</v>
       </c>
       <c r="B11" s="2">
-        <v>5.3029999999999999</v>
+        <v>5.1459999999999999</v>
       </c>
       <c r="C11" s="2">
-        <v>4.5979999999999999</v>
+        <v>4.6180000000000003</v>
       </c>
       <c r="D11" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F11" s="2">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E11" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F11" s="2">
-        <v>4.2000000000000003E-2</v>
-      </c>
       <c r="G11" s="2">
-        <v>5.5E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="H11" t="s">
         <v>5</v>
@@ -829,28 +847,28 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="4">
         <v>4.3579999999999997</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>5.1040000000000001</v>
       </c>
-      <c r="D12" s="2">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E12" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F12" s="2">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F12" s="4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>6.2E-2</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="2">
@@ -861,28 +879,28 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="4">
         <v>6.3780000000000001</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>5.5919999999999996</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.372</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="4">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E13" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F13" s="2">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="F13" s="4">
+        <v>0.374</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="2">
@@ -893,28 +911,28 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="4">
         <v>4.8079999999999998</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>5.9880000000000004</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1.6E-2</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="D14" s="4">
+        <v>0.184</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.151</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.217</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I14" s="2">
@@ -925,28 +943,28 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="4">
         <v>4.931</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>5.798</v>
       </c>
-      <c r="D15" s="2">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.308</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0.377</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="D15" s="4">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="2">
@@ -957,28 +975,28 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="4">
         <v>4.7830000000000004</v>
       </c>
-      <c r="C16" s="2">
-        <v>5.0640000000000001</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="E16" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="F16" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G16" s="2">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="C16" s="4">
+        <v>5.0919999999999996</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G16" s="4">
+        <v>3.9E-2</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="2">
@@ -993,24 +1011,24 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <f>B2-1</f>
+        <f t="shared" ref="B17:C21" si="0">B2-1</f>
         <v>3.62</v>
       </c>
       <c r="C17" s="2">
-        <f>C2-1</f>
+        <f t="shared" si="0"/>
         <v>3.87</v>
       </c>
       <c r="D17" s="2">
-        <v>0.221</v>
+        <v>0.217</v>
       </c>
       <c r="E17" s="2">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F17" s="2">
-        <v>0.19800000000000001</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="G17" s="2">
-        <v>0.245</v>
+        <v>0.24</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
@@ -1027,24 +1045,24 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <f>B3-1</f>
+        <f t="shared" si="0"/>
         <v>5.64</v>
       </c>
       <c r="C18" s="2">
-        <f>C3-1</f>
+        <f t="shared" si="0"/>
         <v>4.28</v>
       </c>
       <c r="D18" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="E18" s="2">
-        <v>1.2999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F18" s="2">
-        <v>0.14099999999999999</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="G18" s="2">
-        <v>0.191</v>
+        <v>0.216</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
@@ -1061,24 +1079,24 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <f>B4-1</f>
+        <f t="shared" si="0"/>
         <v>4.07</v>
       </c>
       <c r="C19" s="2">
-        <f>C4-1</f>
+        <f t="shared" si="0"/>
         <v>4.6100000000000003</v>
       </c>
       <c r="D19" s="2">
-        <v>0.20599999999999999</v>
+        <v>0.193</v>
       </c>
       <c r="E19" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F19" s="2">
-        <v>0.17599999999999999</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="G19" s="2">
-        <v>0.23599999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
@@ -1095,24 +1113,24 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <f>B5-1</f>
+        <f t="shared" si="0"/>
         <v>4.1900000000000004</v>
       </c>
       <c r="C20" s="2">
-        <f>C5-1</f>
+        <f t="shared" si="0"/>
         <v>4.45</v>
       </c>
       <c r="D20" s="2">
-        <v>0.32100000000000001</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="E20" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F20" s="2">
-        <v>0.28799999999999998</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="G20" s="2">
-        <v>0.35399999999999998</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
@@ -1129,24 +1147,24 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <f>B6-1</f>
-        <v>4.04</v>
+        <f t="shared" si="0"/>
+        <v>3.8899999999999997</v>
       </c>
       <c r="C21" s="2">
-        <f>C6-1</f>
-        <v>3.84</v>
+        <f t="shared" si="0"/>
+        <v>3.8600000000000003</v>
       </c>
       <c r="D21" s="2">
-        <v>8.5999999999999993E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E21" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="F21" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="G21" s="2">
-        <v>9.7000000000000003E-2</v>
+        <v>0.108</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
@@ -1159,30 +1177,30 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="2">
-        <f>B2+1</f>
+      <c r="B22" s="4">
+        <f t="shared" ref="B22:C26" si="1">B2+1</f>
         <v>5.62</v>
       </c>
-      <c r="C22" s="2">
-        <f>C2+1</f>
+      <c r="C22" s="4">
+        <f t="shared" si="1"/>
         <v>5.87</v>
       </c>
-      <c r="D22" s="2">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F22" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G22" s="2">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="D22" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G22" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I22" s="2">
@@ -1193,30 +1211,30 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="2">
-        <f>B3+1</f>
+      <c r="B23" s="4">
+        <f t="shared" si="1"/>
         <v>7.64</v>
       </c>
-      <c r="C23" s="2">
-        <f>C3+1</f>
+      <c r="C23" s="4">
+        <f t="shared" si="1"/>
         <v>6.28</v>
       </c>
-      <c r="D23" s="2">
-        <v>0.80100000000000005</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="D23" s="4">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="2">
@@ -1227,30 +1245,30 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="2">
-        <f>B4+1</f>
+      <c r="B24" s="4">
+        <f t="shared" si="1"/>
         <v>6.07</v>
       </c>
-      <c r="C24" s="2">
-        <f>C4+1</f>
+      <c r="C24" s="4">
+        <f t="shared" si="1"/>
         <v>6.61</v>
       </c>
-      <c r="D24" s="2">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E24" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="G24" s="2">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="D24" s="4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F24" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I24" s="2">
@@ -1261,30 +1279,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="2">
-        <f>B5+1</f>
+      <c r="B25" s="4">
+        <f t="shared" si="1"/>
         <v>6.19</v>
       </c>
-      <c r="C25" s="2">
-        <f>C5+1</f>
+      <c r="C25" s="4">
+        <f t="shared" si="1"/>
         <v>6.45</v>
       </c>
-      <c r="D25" s="2">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="F25" s="2">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="D25" s="4">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="F25" s="4">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="2">
@@ -1295,30 +1313,30 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="2">
-        <f>B6+1</f>
-        <v>6.04</v>
-      </c>
-      <c r="C26" s="2">
-        <f>C6+1</f>
-        <v>5.84</v>
-      </c>
-      <c r="D26" s="2">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="E26" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G26" s="2">
-        <v>2.7E-2</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="B26" s="4">
+        <f t="shared" si="1"/>
+        <v>5.89</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="1"/>
+        <v>5.86</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G26" s="4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I26" s="2">

</xml_diff>